<commit_message>
creating sample dataset data
</commit_message>
<xml_diff>
--- a/Sheets/Project-x-Analysts-Model.xlsx
+++ b/Sheets/Project-x-Analysts-Model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardooliveira/Developer/projects-x-analysts/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7E98F1-9306-5D45-A843-5E9DA8FF1DE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A15EE79-0974-7C4E-946E-B5CD72911B7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="28040" windowHeight="16260" activeTab="4" xr2:uid="{37FD05BD-93FE-AB4A-9A22-5B5961D2C4F0}"/>
+    <workbookView xWindow="340" yWindow="500" windowWidth="28040" windowHeight="16260" activeTab="5" xr2:uid="{37FD05BD-93FE-AB4A-9A22-5B5961D2C4F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyst Variables" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Projects Variables" sheetId="4" r:id="rId3"/>
     <sheet name="Projects" sheetId="2" r:id="rId4"/>
     <sheet name="Snapshot Projeto A" sheetId="5" r:id="rId5"/>
+    <sheet name="Planilha6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="69">
   <si>
     <t>identifiação</t>
   </si>
@@ -245,16 +246,38 @@
   </si>
   <si>
     <t>horas</t>
+  </si>
+  <si>
+    <t>Tarefas</t>
+  </si>
+  <si>
+    <t>Analista</t>
+  </si>
+  <si>
+    <t>Quantidade tarefa</t>
+  </si>
+  <si>
+    <t>Pesos</t>
+  </si>
+  <si>
+    <t>Projeto C</t>
+  </si>
+  <si>
+    <t>Projeto B</t>
+  </si>
+  <si>
+    <t>Projeto A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00_);[Red]\(&quot;R$&quot;\ #,###.00\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -269,8 +292,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,8 +340,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -350,11 +419,233 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -391,9 +682,106 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{027C0CC0-B777-F64D-942E-DAA44E278B96}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -845,15 +1233,15 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>c</v>
+        <v>swift</v>
       </c>
       <c r="C3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
-        <v>pleno</v>
+        <v>especialista</v>
       </c>
       <c r="D3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="D3" ca="1">INDEX('Analyst Variables'!$C$2:$C$6, RANDBETWEEN(1,2),1)</f>
-        <v>presencial</v>
+        <v>remoto</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>19</v>
@@ -905,15 +1293,15 @@
       </c>
       <c r="B5" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B5" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>java</v>
+        <v>python</v>
       </c>
       <c r="C5" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
-        <v>especialista</v>
+        <v>trainee</v>
       </c>
       <c r="D5" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="D5" ca="1">INDEX('Analyst Variables'!$C$2:$C$6, RANDBETWEEN(1,2),1)</f>
-        <v>presencial</v>
+        <v>remoto</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>16</v>
@@ -935,11 +1323,11 @@
       </c>
       <c r="B6" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B6" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>objective-c</v>
+        <v>swift</v>
       </c>
       <c r="C6" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
-        <v>trainee</v>
+        <v>especialista</v>
       </c>
       <c r="D6" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="D6" ca="1">INDEX('Analyst Variables'!$C$2:$C$6, RANDBETWEEN(1,2),1)</f>
@@ -965,11 +1353,11 @@
       </c>
       <c r="B7" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B7" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>objective-c</v>
+        <v>swift</v>
       </c>
       <c r="C7" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
-        <v>senior</v>
+        <v>pleno</v>
       </c>
       <c r="D7" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="D7" ca="1">INDEX('Analyst Variables'!$C$2:$C$6, RANDBETWEEN(1,2),1)</f>
@@ -995,7 +1383,7 @@
       </c>
       <c r="B8" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B8" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>python</v>
+        <v>swift</v>
       </c>
       <c r="C8" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
@@ -1012,15 +1400,15 @@
       </c>
       <c r="B9" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B9" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>swift</v>
+        <v>c</v>
       </c>
       <c r="C9" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
-        <v>senior</v>
+        <v>pleno</v>
       </c>
       <c r="D9" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">INDEX('Analyst Variables'!$C$2:$C$6, RANDBETWEEN(1,2),1)</f>
-        <v>remoto</v>
+        <v>presencial</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>46</v>
@@ -1035,7 +1423,7 @@
       </c>
       <c r="B10" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B10" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>python</v>
+        <v>java</v>
       </c>
       <c r="C10" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
@@ -1068,11 +1456,11 @@
       </c>
       <c r="C11" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
-        <v>junior</v>
+        <v>especialista</v>
       </c>
       <c r="D11" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">INDEX('Analyst Variables'!$C$2:$C$6, RANDBETWEEN(1,2),1)</f>
-        <v>remoto</v>
+        <v>presencial</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
@@ -1095,15 +1483,15 @@
       </c>
       <c r="B12" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B12" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>c</v>
+        <v>java</v>
       </c>
       <c r="C12" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
-        <v>senior</v>
+        <v>pleno</v>
       </c>
       <c r="D12" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">INDEX('Analyst Variables'!$C$2:$C$6, RANDBETWEEN(1,2),1)</f>
-        <v>presencial</v>
+        <v>remoto</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>5</v>
@@ -1126,15 +1514,15 @@
       </c>
       <c r="B13" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B13" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>python</v>
+        <v>c</v>
       </c>
       <c r="C13" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
-        <v>senior</v>
+        <v>junior</v>
       </c>
       <c r="D13" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="D13" ca="1">INDEX('Analyst Variables'!$C$2:$C$6, RANDBETWEEN(1,2),1)</f>
-        <v>presencial</v>
+        <v>remoto</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>16</v>
@@ -1157,7 +1545,7 @@
       </c>
       <c r="B14" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B14" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>objective-c</v>
+        <v>java</v>
       </c>
       <c r="C14" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C14" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
@@ -1188,11 +1576,11 @@
       </c>
       <c r="B15" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B15" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>java</v>
+        <v>swift</v>
       </c>
       <c r="C15" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C15" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
-        <v>senior</v>
+        <v>pleno</v>
       </c>
       <c r="D15" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="D15" ca="1">INDEX('Analyst Variables'!$C$2:$C$6, RANDBETWEEN(1,2),1)</f>
@@ -1219,11 +1607,11 @@
       </c>
       <c r="B16" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B16" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>swift</v>
+        <v>c</v>
       </c>
       <c r="C16" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C16" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
-        <v>especialista</v>
+        <v>trainee</v>
       </c>
       <c r="D16" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="D16" ca="1">INDEX('Analyst Variables'!$C$2:$C$6, RANDBETWEEN(1,2),1)</f>
@@ -1237,7 +1625,7 @@
       </c>
       <c r="B17" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B17" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>java</v>
+        <v>python</v>
       </c>
       <c r="C17" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C17" ca="1">INDEX('Analyst Variables'!$B$2:$B$6, RANDBETWEEN(1,5),1)</f>
@@ -1429,14 +1817,14 @@
       </c>
       <c r="C3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>c</v>
+        <v>objective-c</v>
       </c>
       <c r="D3" s="3">
         <v>4000000</v>
       </c>
       <c r="E3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="E3" ca="1">INDEX('Analyst Variables'!$C$2:$C$6, RANDBETWEEN(1,2),1)</f>
-        <v>presencial</v>
+        <v>remoto</v>
       </c>
       <c r="F3" s="2">
         <v>200</v>
@@ -1459,7 +1847,7 @@
       </c>
       <c r="C4" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>swift</v>
+        <v>objective-c</v>
       </c>
       <c r="D4" s="3">
         <v>1000000</v>
@@ -1489,14 +1877,14 @@
       </c>
       <c r="C5" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">INDEX('Analyst Variables'!$A$2:$A$6, RANDBETWEEN(1,5),1)</f>
-        <v>swift</v>
+        <v>objective-c</v>
       </c>
       <c r="D5" s="3">
         <v>2000000</v>
       </c>
       <c r="E5" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="E5" ca="1">INDEX('Analyst Variables'!$C$2:$C$6, RANDBETWEEN(1,2),1)</f>
-        <v>remoto</v>
+        <v>presencial</v>
       </c>
       <c r="F5" s="2">
         <v>700</v>
@@ -1544,7 +1932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2DF3F6-B09F-354C-BDA3-8DF045C24F33}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -1992,4 +2380,344 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C0DFED-83F7-D045-8406-2527F2003C0C}">
+  <dimension ref="A3:P19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="16"/>
+    <col min="2" max="2" width="5" style="16" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" style="16" customWidth="1"/>
+    <col min="4" max="8" width="4.33203125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" style="16" customWidth="1"/>
+    <col min="10" max="10" width="5.1640625" style="16" customWidth="1"/>
+    <col min="11" max="15" width="9" style="16"/>
+    <col min="16" max="16" width="17" style="16" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="50">
+        <v>6</v>
+      </c>
+      <c r="C4" s="49">
+        <v>8</v>
+      </c>
+      <c r="D4" s="48">
+        <v>11</v>
+      </c>
+      <c r="E4" s="47">
+        <v>2</v>
+      </c>
+      <c r="F4" s="46">
+        <v>14</v>
+      </c>
+      <c r="G4" s="45">
+        <v>7</v>
+      </c>
+      <c r="H4" s="44">
+        <v>5</v>
+      </c>
+      <c r="I4" s="43">
+        <v>13</v>
+      </c>
+      <c r="J4" s="42">
+        <v>1</v>
+      </c>
+      <c r="P4" s="41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="40">
+        <v>20</v>
+      </c>
+      <c r="C5" s="39">
+        <v>75</v>
+      </c>
+      <c r="D5" s="38">
+        <v>45</v>
+      </c>
+      <c r="E5" s="37">
+        <v>12</v>
+      </c>
+      <c r="F5" s="36">
+        <v>85</v>
+      </c>
+      <c r="G5" s="35">
+        <v>180</v>
+      </c>
+      <c r="H5" s="34">
+        <v>147</v>
+      </c>
+      <c r="I5" s="33">
+        <v>84</v>
+      </c>
+      <c r="J5" s="32">
+        <v>45</v>
+      </c>
+      <c r="P5" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="30">
+        <v>3</v>
+      </c>
+      <c r="C7" s="29">
+        <v>12</v>
+      </c>
+      <c r="D7" s="28">
+        <v>9</v>
+      </c>
+      <c r="E7" s="30">
+        <v>5</v>
+      </c>
+      <c r="F7" s="29">
+        <v>6</v>
+      </c>
+      <c r="G7" s="28">
+        <v>15</v>
+      </c>
+      <c r="H7" s="30">
+        <v>13</v>
+      </c>
+      <c r="I7" s="29">
+        <v>2</v>
+      </c>
+      <c r="J7" s="28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="26">
+        <v>8</v>
+      </c>
+      <c r="C8" s="25">
+        <v>90</v>
+      </c>
+      <c r="D8" s="24">
+        <v>41</v>
+      </c>
+      <c r="E8" s="26">
+        <v>42</v>
+      </c>
+      <c r="F8" s="25">
+        <v>54</v>
+      </c>
+      <c r="G8" s="24">
+        <v>129</v>
+      </c>
+      <c r="H8" s="26">
+        <v>145</v>
+      </c>
+      <c r="I8" s="25">
+        <v>11</v>
+      </c>
+      <c r="J8" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="30">
+        <v>1</v>
+      </c>
+      <c r="C10" s="29">
+        <v>8</v>
+      </c>
+      <c r="D10" s="28">
+        <v>11</v>
+      </c>
+      <c r="E10" s="30">
+        <v>2</v>
+      </c>
+      <c r="F10" s="29">
+        <v>14</v>
+      </c>
+      <c r="G10" s="28">
+        <v>9</v>
+      </c>
+      <c r="H10" s="30">
+        <v>5</v>
+      </c>
+      <c r="I10" s="29">
+        <v>15</v>
+      </c>
+      <c r="J10" s="28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="26">
+        <v>12</v>
+      </c>
+      <c r="C11" s="25">
+        <v>18</v>
+      </c>
+      <c r="D11" s="24">
+        <v>99</v>
+      </c>
+      <c r="E11" s="26">
+        <v>22</v>
+      </c>
+      <c r="F11" s="25">
+        <v>28</v>
+      </c>
+      <c r="G11" s="24">
+        <v>94</v>
+      </c>
+      <c r="H11" s="26">
+        <v>1</v>
+      </c>
+      <c r="I11" s="25">
+        <v>195</v>
+      </c>
+      <c r="J11" s="24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="30">
+        <v>3</v>
+      </c>
+      <c r="C13" s="29">
+        <v>11</v>
+      </c>
+      <c r="D13" s="28">
+        <v>13</v>
+      </c>
+      <c r="E13" s="30">
+        <v>2</v>
+      </c>
+      <c r="F13" s="29">
+        <v>6</v>
+      </c>
+      <c r="G13" s="28">
+        <v>9</v>
+      </c>
+      <c r="H13" s="30">
+        <v>7</v>
+      </c>
+      <c r="I13" s="29">
+        <v>14</v>
+      </c>
+      <c r="J13" s="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="26">
+        <v>56</v>
+      </c>
+      <c r="C14" s="25">
+        <v>4</v>
+      </c>
+      <c r="D14" s="24">
+        <v>42</v>
+      </c>
+      <c r="E14" s="26">
+        <v>111</v>
+      </c>
+      <c r="F14" s="25">
+        <v>36</v>
+      </c>
+      <c r="G14" s="24">
+        <v>12</v>
+      </c>
+      <c r="H14" s="26">
+        <v>8</v>
+      </c>
+      <c r="I14" s="25">
+        <v>55</v>
+      </c>
+      <c r="J14" s="24">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="23"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="22"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="20"/>
+    </row>
+    <row r="19" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="19"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>